<commit_message>
temp occ traits saved for ms resubmission
</commit_message>
<xml_diff>
--- a/data/tempocctraits.xlsx
+++ b/data/tempocctraits.xlsx
@@ -9,15 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="combined" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="trait_mod_output_arcsine" localSheetId="0">combined!$F$2:$I$15</definedName>
+    <definedName name="trait_mod_output_arcsine" localSheetId="1">Sheet1!$F$2:$G$15</definedName>
     <definedName name="trait_mod_output_logit_1" localSheetId="0">combined!$B$2:$E$15</definedName>
+    <definedName name="trait_mod_output_logit_1" localSheetId="1">Sheet1!$D$2:$E$15</definedName>
     <definedName name="trait_mod_output_og_logit" localSheetId="0">combined!$A$2:$O$15</definedName>
+    <definedName name="trait_mod_output_og_logit" localSheetId="1">Sheet1!$A$2:$C$15</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +46,19 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="trait_mod_output_logit" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" name="trait_mod_output_arcsine1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Git\Biotic-Interactions\data\trait_mod_output_arcsine.txt" delimited="0">
+      <textFields count="6">
+        <textField/>
+        <textField position="24"/>
+        <textField position="35"/>
+        <textField position="46"/>
+        <textField position="54"/>
+        <textField position="63"/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="trait_mod_output_logit" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Git\Biotic-Interactions\data\trait_mod_output_logit.txt" delimited="0">
       <textFields count="6">
         <textField/>
@@ -54,7 +70,31 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="trait_mod_output_og_logit" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" name="trait_mod_output_logit1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Git\Biotic-Interactions\data\trait_mod_output_logit.txt" delimited="0">
+      <textFields count="6">
+        <textField/>
+        <textField position="24"/>
+        <textField position="35"/>
+        <textField position="46"/>
+        <textField position="54"/>
+        <textField position="63"/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="trait_mod_output_og_logit" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Git\Biotic-Interactions\data\trait_mod_output_og_logit.txt" delimited="0">
+      <textFields count="6">
+        <textField/>
+        <textField position="24"/>
+        <textField position="35"/>
+        <textField position="46"/>
+        <textField position="54"/>
+        <textField position="63"/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="trait_mod_output_og_logit1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Git\Biotic-Interactions\data\trait_mod_output_og_logit.txt" delimited="0">
       <textFields count="6">
         <textField/>
@@ -70,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>Estimate</t>
   </si>
@@ -157,16 +197,29 @@
   </si>
   <si>
     <t>Pr(&gt;|t|) - arcsine</t>
+  </si>
+  <si>
+    <t>Including median occupancy; logit transform</t>
+  </si>
+  <si>
+    <t>Including median occupancy; arcsin transform</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Original results; logit transform</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +232,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -207,7 +265,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -215,11 +273,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -230,6 +329,31 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -248,15 +372,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="trait_mod_output_logit_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="trait_mod_output_og_logit" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="trait_mod_output_og_logit" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="trait_mod_output_arcsine" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="trait_mod_output_arcsine" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="trait_mod_output_logit_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="trait_mod_output_logit_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="trait_mod_output_arcsine" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="trait_mod_output_og_logit" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -524,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +826,7 @@
       <c r="D5" s="6">
         <v>8.0719999999999992</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="8">
         <v>1.7400000000000001E-15</v>
       </c>
       <c r="F5" s="7">
@@ -764,7 +900,7 @@
       <c r="D7" s="6">
         <v>-3.8039999999999998</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="8">
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="F7" s="7">
@@ -1092,7 +1228,7 @@
       <c r="D15" s="6">
         <v>3.8239999999999998</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="8">
         <v>1.3799999999999999E-4</v>
       </c>
       <c r="F15" s="7">
@@ -1124,4 +1260,365 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="14" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13"/>
+      <c r="B1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="11">
+        <v>15.9996098</v>
+      </c>
+      <c r="C3" s="12">
+        <v>2.19E-13</v>
+      </c>
+      <c r="D3" s="11">
+        <v>19.509011000000001</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11">
+        <v>4.8540000000000001</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="11">
+        <v>-2.3296407000000001</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="11">
+        <v>-2.880493</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="11">
+        <v>-0.57030000000000003</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11">
+        <v>2.3747796999999999</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1.7400000000000001E-15</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.41689999999999999</v>
+      </c>
+      <c r="G5" s="12">
+        <v>5.9599999999999998E-13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="11">
+        <v>4.9043499999999997E-2</v>
+      </c>
+      <c r="C6" s="11">
+        <v>7.6400000000000003E-4</v>
+      </c>
+      <c r="D6" s="11">
+        <v>4.1703499999999998E-2</v>
+      </c>
+      <c r="E6" s="11">
+        <v>3.3240000000000001E-3</v>
+      </c>
+      <c r="F6" s="11">
+        <v>8.0440000000000008E-3</v>
+      </c>
+      <c r="G6" s="11">
+        <v>3.591E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="11">
+        <v>-9.3626999999999998E-3</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2.0129000000000001E-2</v>
+      </c>
+      <c r="D7" s="11">
+        <v>-1.51434E-2</v>
+      </c>
+      <c r="E7" s="12">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="F7" s="11">
+        <v>-3.4759999999999999E-3</v>
+      </c>
+      <c r="G7" s="12">
+        <v>7.8399999999999995E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11">
+        <v>1.06243E-2</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.120033</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2.3181799999999999E-2</v>
+      </c>
+      <c r="E8" s="11">
+        <v>7.0699999999999995E-4</v>
+      </c>
+      <c r="F8" s="11">
+        <v>4.5640000000000003E-3</v>
+      </c>
+      <c r="G8" s="11">
+        <v>6.0800000000000003E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="12">
+        <v>3.589E-4</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.37922499999999998</v>
+      </c>
+      <c r="D9" s="11">
+        <v>4.6880000000000001E-4</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.23828299999999999</v>
+      </c>
+      <c r="F9" s="11">
+        <v>2.5680000000000001E-5</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.73970899999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="11">
+        <v>-2.0131505000000001</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.269507</v>
+      </c>
+      <c r="D10" s="11">
+        <v>-4.5671888000000003</v>
+      </c>
+      <c r="E10" s="11">
+        <v>1.137E-2</v>
+      </c>
+      <c r="F10" s="11">
+        <v>-1.0640000000000001</v>
+      </c>
+      <c r="G10" s="11">
+        <v>2.4390000000000002E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1.0039781999999999</v>
+      </c>
+      <c r="C11" s="11">
+        <v>6.0400000000000004E-4</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0.67589580000000005</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1.8678E-2</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0.18490000000000001</v>
+      </c>
+      <c r="G11" s="11">
+        <v>9.5E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="11">
+        <v>0.65705259999999999</v>
+      </c>
+      <c r="C12" s="11">
+        <v>2.4990999999999999E-2</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0.51955110000000004</v>
+      </c>
+      <c r="E12" s="11">
+        <v>6.8964999999999999E-2</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0.15870000000000001</v>
+      </c>
+      <c r="G12" s="11">
+        <v>4.3299999999999996E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11">
+        <v>-0.38520569999999998</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0.32131599999999999</v>
+      </c>
+      <c r="D13" s="11">
+        <v>-0.60181609999999996</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.11239</v>
+      </c>
+      <c r="F13" s="11">
+        <v>-0.11169999999999999</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0.12967300000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="11">
+        <v>-0.7328538</v>
+      </c>
+      <c r="C14" s="12">
+        <v>7.7600000000000002E-5</v>
+      </c>
+      <c r="D14" s="11">
+        <v>-0.45834150000000001</v>
+      </c>
+      <c r="E14" s="11">
+        <v>1.2406E-2</v>
+      </c>
+      <c r="F14" s="11">
+        <v>-5.28E-2</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0.138269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0.60133550000000002</v>
+      </c>
+      <c r="C15" s="12">
+        <v>2.5299999999999999E-6</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0.47688150000000001</v>
+      </c>
+      <c r="E15" s="12">
+        <v>1.3799999999999999E-4</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0.1065</v>
+      </c>
+      <c r="G15" s="12">
+        <v>1.24E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>